<commit_message>
Added constraints for register panel
</commit_message>
<xml_diff>
--- a/attendance_report_03_2025.xlsx
+++ b/attendance_report_03_2025.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,7 +463,22 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Thejas L</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>4GH16EC054</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>